<commit_message>
update add score more
</commit_message>
<xml_diff>
--- a/6.xlsx
+++ b/6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shegg\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Space\java\project-do-an-chuyen-nganh\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -416,7 +416,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +452,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update add score from excel
</commit_message>
<xml_diff>
--- a/6.xlsx
+++ b/6.xlsx
@@ -416,7 +416,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +452,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>